<commit_message>
"Tailwind calculation - done!"
</commit_message>
<xml_diff>
--- a/Tailwind-Traders-Sales.xlsx
+++ b/Tailwind-Traders-Sales.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maharajs\Desktop\Course 7\Module 4\Capstone Screenshots\1_Prepare sales Excel data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Courses\Coursera\Microsoft Power BI Data Analyst Professional Certificate\Microsoft Power BI Data Analyst Professional Certificate\POWER BI\Capstone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE9546F-D460-4117-9A7C-A2E2343B9D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66550900-4719-440E-B1FC-67B051E1C895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sales!$A$1:$V$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sales!$A$1:$Y$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="465">
   <si>
     <t xml:space="preserve"> OrderID </t>
   </si>
@@ -1425,6 +1425,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Country ID</t>
+  </si>
+  <si>
+    <t>Gross Revenue</t>
+  </si>
+  <si>
+    <t>Total Tax</t>
+  </si>
+  <si>
+    <t>Net Revenue</t>
   </si>
 </sst>
 </file>
@@ -1743,26 +1752,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.81640625" customWidth="1"/>
-    <col min="18" max="18" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="10" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1785,52 +1794,61 @@
         <v>436</v>
       </c>
       <c r="H1" t="s">
+        <v>462</v>
+      </c>
+      <c r="I1" t="s">
+        <v>463</v>
+      </c>
+      <c r="J1" t="s">
+        <v>464</v>
+      </c>
+      <c r="K1" t="s">
         <v>406</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>461</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1024</v>
       </c>
@@ -1852,53 +1870,65 @@
       <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <f>E2*G2</f>
+        <v>120</v>
+      </c>
+      <c r="I2">
+        <f>F2*G2</f>
+        <v>16.8</v>
+      </c>
+      <c r="J2">
+        <f>H2-I2</f>
+        <v>103.2</v>
+      </c>
+      <c r="K2" t="s">
         <v>312</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>320</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>22</v>
       </c>
-      <c r="S2">
+      <c r="V2">
         <v>46575</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>1112222</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>23</v>
       </c>
-      <c r="V2">
+      <c r="Y2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1025</v>
       </c>
@@ -1920,53 +1950,65 @@
       <c r="G3">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <f t="shared" ref="H3:H55" si="0">E3*G3</f>
+        <v>105</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I55" si="1">F3*G3</f>
+        <v>7.3500000000000005</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J55" si="2">H3-I3</f>
+        <v>97.65</v>
+      </c>
+      <c r="K3" t="s">
         <v>315</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>28</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
         <v>150</v>
       </c>
-      <c r="O3">
+      <c r="R3">
         <v>5</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>30</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>31</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>2223333</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>33</v>
       </c>
-      <c r="V3">
+      <c r="Y3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1026</v>
       </c>
@@ -1988,53 +2030,65 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>17.5</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>232.5</v>
+      </c>
+      <c r="K4" t="s">
         <v>318</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>38</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>85</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>39</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>40</v>
       </c>
-      <c r="S4">
+      <c r="V4">
         <v>75008</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>3334444</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>41</v>
       </c>
-      <c r="V4">
+      <c r="Y4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1027</v>
       </c>
@@ -2056,53 +2110,65 @@
       <c r="G5">
         <v>5</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5.25</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>69.75</v>
+      </c>
+      <c r="K5" t="s">
         <v>312</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>45</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>190</v>
       </c>
-      <c r="O5">
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>46</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="T5" t="s">
         <v>47</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>48</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>10178</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>4445555</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>49</v>
       </c>
-      <c r="V5">
+      <c r="Y5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1028</v>
       </c>
@@ -2124,53 +2190,65 @@
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>15.4</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>204.6</v>
+      </c>
+      <c r="K6" t="s">
         <v>323</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>52</v>
       </c>
-      <c r="L6" t="s">
+      <c r="O6" t="s">
         <v>18</v>
       </c>
-      <c r="M6" t="s">
+      <c r="P6" t="s">
         <v>53</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>310</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>54</v>
       </c>
-      <c r="R6" t="s">
+      <c r="U6" t="s">
         <v>55</v>
       </c>
-      <c r="S6">
+      <c r="V6">
         <v>28014</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>5556666</v>
       </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
         <v>56</v>
       </c>
-      <c r="V6">
+      <c r="Y6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1029</v>
       </c>
@@ -2192,53 +2270,65 @@
       <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>139.5</v>
+      </c>
+      <c r="K7" t="s">
         <v>326</v>
       </c>
-      <c r="I7" t="s">
+      <c r="L7" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="K7" t="s">
+      <c r="N7" t="s">
         <v>59</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
         <v>27</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" t="s">
         <v>60</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <v>210</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <v>2</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
         <v>61</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>62</v>
       </c>
-      <c r="R7" t="s">
+      <c r="U7" t="s">
         <v>63</v>
       </c>
-      <c r="S7">
+      <c r="V7">
         <v>185</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>6667777</v>
       </c>
-      <c r="U7" t="s">
+      <c r="X7" t="s">
         <v>64</v>
       </c>
-      <c r="V7">
+      <c r="Y7">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1030</v>
       </c>
@@ -2260,53 +2350,65 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>14.7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>35.299999999999997</v>
+      </c>
+      <c r="K8" t="s">
         <v>329</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="K8" t="s">
+      <c r="N8" t="s">
         <v>17</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>37</v>
       </c>
-      <c r="M8" t="s">
+      <c r="P8" t="s">
         <v>67</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <v>255</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>3</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" t="s">
         <v>46</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="T8" t="s">
         <v>68</v>
       </c>
-      <c r="R8" t="s">
+      <c r="U8" t="s">
         <v>69</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>110001</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>7778888</v>
       </c>
-      <c r="U8" t="s">
+      <c r="X8" t="s">
         <v>70</v>
       </c>
-      <c r="V8">
+      <c r="Y8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1031</v>
       </c>
@@ -2328,53 +2430,65 @@
       <c r="G9">
         <v>3</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>251.1</v>
+      </c>
+      <c r="K9" t="s">
         <v>332</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="L9" t="s">
+      <c r="O9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" t="s">
+      <c r="P9" t="s">
         <v>73</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <v>265</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>2</v>
       </c>
-      <c r="P9" t="s">
+      <c r="S9" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="T9" t="s">
         <v>74</v>
       </c>
-      <c r="R9" t="s">
+      <c r="U9" t="s">
         <v>75</v>
       </c>
-      <c r="S9" t="s">
+      <c r="V9" t="s">
         <v>76</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>8889999</v>
       </c>
-      <c r="U9" t="s">
+      <c r="X9" t="s">
         <v>77</v>
       </c>
-      <c r="V9">
+      <c r="Y9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1032</v>
       </c>
@@ -2396,53 +2510,65 @@
       <c r="G10">
         <v>2</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>25.2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>334.8</v>
+      </c>
+      <c r="K10" t="s">
         <v>312</v>
       </c>
-      <c r="I10" t="s">
+      <c r="L10" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="K10" t="s">
+      <c r="N10" t="s">
         <v>36</v>
       </c>
-      <c r="L10" t="s">
+      <c r="O10" t="s">
         <v>44</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
         <v>80</v>
       </c>
-      <c r="N10">
+      <c r="Q10">
         <v>330</v>
       </c>
-      <c r="O10">
+      <c r="R10">
         <v>1</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="T10" t="s">
         <v>81</v>
       </c>
-      <c r="R10" t="s">
+      <c r="U10" t="s">
         <v>82</v>
       </c>
-      <c r="S10">
+      <c r="V10">
         <v>2000</v>
       </c>
-      <c r="T10">
+      <c r="W10">
         <v>9990000</v>
       </c>
-      <c r="U10" t="s">
+      <c r="X10" t="s">
         <v>83</v>
       </c>
-      <c r="V10">
+      <c r="Y10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1033</v>
       </c>
@@ -2464,53 +2590,65 @@
       <c r="G11">
         <v>6</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="K11" t="s">
         <v>329</v>
       </c>
-      <c r="I11" t="s">
+      <c r="L11" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K11" t="s">
+      <c r="N11" t="s">
         <v>86</v>
       </c>
-      <c r="L11" t="s">
+      <c r="O11" t="s">
         <v>18</v>
       </c>
-      <c r="M11" t="s">
+      <c r="P11" t="s">
         <v>28</v>
       </c>
-      <c r="N11">
+      <c r="Q11">
         <v>500</v>
       </c>
-      <c r="O11">
+      <c r="R11">
         <v>1</v>
       </c>
-      <c r="P11" t="s">
+      <c r="S11" t="s">
         <v>61</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="T11" t="s">
         <v>87</v>
       </c>
-      <c r="R11" t="s">
+      <c r="U11" t="s">
         <v>88</v>
       </c>
-      <c r="S11" t="s">
+      <c r="V11" t="s">
         <v>89</v>
       </c>
-      <c r="T11">
+      <c r="W11">
         <v>1497911</v>
       </c>
-      <c r="U11" t="s">
+      <c r="X11" t="s">
         <v>90</v>
       </c>
-      <c r="V11">
+      <c r="Y11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1034</v>
       </c>
@@ -2532,53 +2670,65 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="K12" t="s">
         <v>326</v>
       </c>
-      <c r="I12" t="s">
+      <c r="L12" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="K12" t="s">
+      <c r="N12" t="s">
         <v>52</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>27</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" t="s">
         <v>67</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <v>220</v>
       </c>
-      <c r="O12">
+      <c r="R12">
         <v>2</v>
       </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>20</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="T12" t="s">
         <v>93</v>
       </c>
-      <c r="R12" t="s">
+      <c r="U12" t="s">
         <v>94</v>
       </c>
-      <c r="S12">
+      <c r="V12">
         <v>67890</v>
       </c>
-      <c r="T12">
+      <c r="W12">
         <v>1122334</v>
       </c>
-      <c r="U12" t="s">
+      <c r="X12" t="s">
         <v>95</v>
       </c>
-      <c r="V12">
+      <c r="Y12">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1035</v>
       </c>
@@ -2600,53 +2750,65 @@
       <c r="G13">
         <v>4</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>186</v>
+      </c>
+      <c r="K13" t="s">
         <v>315</v>
       </c>
-      <c r="I13" t="s">
+      <c r="L13" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="K13" t="s">
+      <c r="N13" t="s">
         <v>59</v>
       </c>
-      <c r="L13" t="s">
+      <c r="O13" t="s">
         <v>37</v>
       </c>
-      <c r="M13" t="s">
+      <c r="P13" t="s">
         <v>53</v>
       </c>
-      <c r="N13">
+      <c r="Q13">
         <v>150</v>
       </c>
-      <c r="O13">
+      <c r="R13">
         <v>4</v>
       </c>
-      <c r="P13" t="s">
+      <c r="S13" t="s">
         <v>46</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="T13" t="s">
         <v>98</v>
       </c>
-      <c r="R13" t="s">
+      <c r="U13" t="s">
         <v>99</v>
       </c>
-      <c r="S13">
+      <c r="V13">
         <v>12345</v>
       </c>
-      <c r="T13">
+      <c r="W13">
         <v>2233445</v>
       </c>
-      <c r="U13" t="s">
+      <c r="X13" t="s">
         <v>100</v>
       </c>
-      <c r="V13">
+      <c r="Y13">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1036</v>
       </c>
@@ -2668,53 +2830,65 @@
       <c r="G14">
         <v>5</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="K14" t="s">
         <v>323</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="K14" t="s">
+      <c r="N14" t="s">
         <v>86</v>
       </c>
-      <c r="L14" t="s">
+      <c r="O14" t="s">
         <v>44</v>
       </c>
-      <c r="M14" t="s">
+      <c r="P14" t="s">
         <v>38</v>
       </c>
-      <c r="N14">
+      <c r="Q14">
         <v>90</v>
       </c>
-      <c r="O14">
+      <c r="R14">
         <v>1</v>
       </c>
-      <c r="P14" t="s">
+      <c r="S14" t="s">
         <v>29</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="T14" t="s">
         <v>103</v>
       </c>
-      <c r="R14" t="s">
+      <c r="U14" t="s">
         <v>104</v>
       </c>
-      <c r="S14">
+      <c r="V14">
         <v>34567</v>
       </c>
-      <c r="T14">
+      <c r="W14">
         <v>3344556</v>
       </c>
-      <c r="U14" t="s">
+      <c r="X14" t="s">
         <v>105</v>
       </c>
-      <c r="V14">
+      <c r="Y14">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1037</v>
       </c>
@@ -2736,53 +2910,65 @@
       <c r="G15">
         <v>3</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>111.6</v>
+      </c>
+      <c r="K15" t="s">
         <v>345</v>
       </c>
-      <c r="I15" t="s">
+      <c r="L15" t="s">
         <v>107</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="K15" t="s">
+      <c r="N15" t="s">
         <v>17</v>
       </c>
-      <c r="L15" t="s">
+      <c r="O15" t="s">
         <v>27</v>
       </c>
-      <c r="M15" t="s">
+      <c r="P15" t="s">
         <v>28</v>
       </c>
-      <c r="N15">
+      <c r="Q15">
         <v>320</v>
       </c>
-      <c r="O15">
+      <c r="R15">
         <v>5</v>
       </c>
-      <c r="P15" t="s">
+      <c r="S15" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="T15" t="s">
         <v>108</v>
       </c>
-      <c r="R15" t="s">
+      <c r="U15" t="s">
         <v>109</v>
       </c>
-      <c r="S15">
+      <c r="V15">
         <v>45678</v>
       </c>
-      <c r="T15">
+      <c r="W15">
         <v>4455667</v>
       </c>
-      <c r="U15" t="s">
+      <c r="X15" t="s">
         <v>110</v>
       </c>
-      <c r="V15">
+      <c r="Y15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1038</v>
       </c>
@@ -2804,53 +2990,65 @@
       <c r="G16">
         <v>4</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>12.6</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>167.4</v>
+      </c>
+      <c r="K16" t="s">
         <v>318</v>
       </c>
-      <c r="I16" t="s">
+      <c r="L16" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="K16" t="s">
+      <c r="N16" t="s">
         <v>26</v>
       </c>
-      <c r="L16" t="s">
+      <c r="O16" t="s">
         <v>44</v>
       </c>
-      <c r="M16" t="s">
+      <c r="P16" t="s">
         <v>73</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <v>185</v>
       </c>
-      <c r="O16">
+      <c r="R16">
         <v>5</v>
       </c>
-      <c r="P16" t="s">
+      <c r="S16" t="s">
         <v>20</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="T16" t="s">
         <v>113</v>
       </c>
-      <c r="R16" t="s">
+      <c r="U16" t="s">
         <v>114</v>
       </c>
-      <c r="S16">
+      <c r="V16">
         <v>56789</v>
       </c>
-      <c r="T16">
+      <c r="W16">
         <v>5566778</v>
       </c>
-      <c r="U16" t="s">
+      <c r="X16" t="s">
         <v>115</v>
       </c>
-      <c r="V16">
+      <c r="Y16">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1039</v>
       </c>
@@ -2872,53 +3070,65 @@
       <c r="G17">
         <v>2</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>11.2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>148.80000000000001</v>
+      </c>
+      <c r="K17" t="s">
         <v>323</v>
       </c>
-      <c r="I17" t="s">
+      <c r="L17" t="s">
         <v>117</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="K17" t="s">
+      <c r="N17" t="s">
         <v>36</v>
       </c>
-      <c r="L17" t="s">
+      <c r="O17" t="s">
         <v>18</v>
       </c>
-      <c r="M17" t="s">
+      <c r="P17" t="s">
         <v>19</v>
       </c>
-      <c r="N17">
+      <c r="Q17">
         <v>215</v>
       </c>
-      <c r="O17">
+      <c r="R17">
         <v>1</v>
       </c>
-      <c r="P17" t="s">
+      <c r="S17" t="s">
         <v>46</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="T17" t="s">
         <v>118</v>
       </c>
-      <c r="R17" t="s">
+      <c r="U17" t="s">
         <v>119</v>
       </c>
-      <c r="S17">
+      <c r="V17">
         <v>67890</v>
       </c>
-      <c r="T17">
+      <c r="W17">
         <v>6677889</v>
       </c>
-      <c r="U17" t="s">
+      <c r="X17" t="s">
         <v>120</v>
       </c>
-      <c r="V17">
+      <c r="Y17">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1040</v>
       </c>
@@ -2940,53 +3150,65 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>186</v>
+      </c>
+      <c r="K18" t="s">
         <v>332</v>
       </c>
-      <c r="I18" t="s">
+      <c r="L18" t="s">
         <v>122</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K18" t="s">
+      <c r="N18" t="s">
         <v>17</v>
       </c>
-      <c r="L18" t="s">
+      <c r="O18" t="s">
         <v>18</v>
       </c>
-      <c r="M18" t="s">
+      <c r="P18" t="s">
         <v>67</v>
       </c>
-      <c r="N18">
+      <c r="Q18">
         <v>240</v>
       </c>
-      <c r="O18">
+      <c r="R18">
         <v>5</v>
       </c>
-      <c r="P18" t="s">
+      <c r="S18" t="s">
         <v>61</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="T18" t="s">
         <v>123</v>
       </c>
-      <c r="R18" t="s">
+      <c r="U18" t="s">
         <v>124</v>
       </c>
-      <c r="S18">
+      <c r="V18">
         <v>78901</v>
       </c>
-      <c r="T18">
+      <c r="W18">
         <v>7788990</v>
       </c>
-      <c r="U18" t="s">
+      <c r="X18" t="s">
         <v>125</v>
       </c>
-      <c r="V18">
+      <c r="Y18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1041</v>
       </c>
@@ -3008,53 +3230,65 @@
       <c r="G19">
         <v>3</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>13.649999999999999</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>181.35</v>
+      </c>
+      <c r="K19" t="s">
         <v>345</v>
       </c>
-      <c r="I19" t="s">
+      <c r="L19" t="s">
         <v>127</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="K19" t="s">
+      <c r="N19" t="s">
         <v>26</v>
       </c>
-      <c r="L19" t="s">
+      <c r="O19" t="s">
         <v>27</v>
       </c>
-      <c r="M19" t="s">
+      <c r="P19" t="s">
         <v>28</v>
       </c>
-      <c r="N19">
+      <c r="Q19">
         <v>165</v>
       </c>
-      <c r="O19">
+      <c r="R19">
         <v>5</v>
       </c>
-      <c r="P19" t="s">
+      <c r="S19" t="s">
         <v>29</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="T19" t="s">
         <v>128</v>
       </c>
-      <c r="R19" t="s">
+      <c r="U19" t="s">
         <v>129</v>
       </c>
-      <c r="S19">
+      <c r="V19">
         <v>89012</v>
       </c>
-      <c r="T19">
+      <c r="W19">
         <v>8899001</v>
       </c>
-      <c r="U19" t="s">
+      <c r="X19" t="s">
         <v>130</v>
       </c>
-      <c r="V19">
+      <c r="Y19">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1042</v>
       </c>
@@ -3076,53 +3310,65 @@
       <c r="G20">
         <v>2</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>15.4</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>204.6</v>
+      </c>
+      <c r="K20" t="s">
         <v>318</v>
       </c>
-      <c r="I20" t="s">
+      <c r="L20" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="K20" t="s">
+      <c r="N20" t="s">
         <v>36</v>
       </c>
-      <c r="L20" t="s">
+      <c r="O20" t="s">
         <v>37</v>
       </c>
-      <c r="M20" t="s">
+      <c r="P20" t="s">
         <v>53</v>
       </c>
-      <c r="N20">
+      <c r="Q20">
         <v>300</v>
       </c>
-      <c r="O20">
+      <c r="R20">
         <v>1</v>
       </c>
-      <c r="P20" t="s">
+      <c r="S20" t="s">
         <v>61</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="T20" t="s">
         <v>133</v>
       </c>
-      <c r="R20" t="s">
+      <c r="U20" t="s">
         <v>134</v>
       </c>
-      <c r="S20">
+      <c r="V20">
         <v>90123</v>
       </c>
-      <c r="T20">
+      <c r="W20">
         <v>9900112</v>
       </c>
-      <c r="U20" t="s">
+      <c r="X20" t="s">
         <v>135</v>
       </c>
-      <c r="V20">
+      <c r="Y20">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1043</v>
       </c>
@@ -3144,53 +3390,65 @@
       <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>6.65</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>88.35</v>
+      </c>
+      <c r="K21" t="s">
         <v>318</v>
       </c>
-      <c r="I21" t="s">
+      <c r="L21" t="s">
         <v>137</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="K21" t="s">
+      <c r="N21" t="s">
         <v>17</v>
       </c>
-      <c r="L21" t="s">
+      <c r="O21" t="s">
         <v>44</v>
       </c>
-      <c r="M21" t="s">
+      <c r="P21" t="s">
         <v>45</v>
       </c>
-      <c r="N21">
+      <c r="Q21">
         <v>270</v>
       </c>
-      <c r="O21">
+      <c r="R21">
         <v>2</v>
       </c>
-      <c r="P21" t="s">
+      <c r="S21" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="T21" t="s">
         <v>138</v>
       </c>
-      <c r="R21" t="s">
+      <c r="U21" t="s">
         <v>139</v>
       </c>
-      <c r="S21">
+      <c r="V21">
         <v>12378</v>
       </c>
-      <c r="T21">
+      <c r="W21">
         <v>10121314</v>
       </c>
-      <c r="U21" t="s">
+      <c r="X21" t="s">
         <v>140</v>
       </c>
-      <c r="V21">
+      <c r="Y21">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1044</v>
       </c>
@@ -3212,53 +3470,65 @@
       <c r="G22">
         <v>3</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>27.299999999999997</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>362.7</v>
+      </c>
+      <c r="K22" t="s">
         <v>360</v>
       </c>
-      <c r="I22" t="s">
+      <c r="L22" t="s">
         <v>142</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K22" t="s">
+      <c r="N22" t="s">
         <v>52</v>
       </c>
-      <c r="L22" t="s">
+      <c r="O22" t="s">
         <v>18</v>
       </c>
-      <c r="M22" t="s">
+      <c r="P22" t="s">
         <v>73</v>
       </c>
-      <c r="N22">
+      <c r="Q22">
         <v>315</v>
       </c>
-      <c r="O22">
+      <c r="R22">
         <v>3</v>
       </c>
-      <c r="P22" t="s">
+      <c r="S22" t="s">
         <v>29</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="T22" t="s">
         <v>143</v>
       </c>
-      <c r="R22" t="s">
+      <c r="U22" t="s">
         <v>144</v>
       </c>
-      <c r="S22">
+      <c r="V22">
         <v>23489</v>
       </c>
-      <c r="T22">
+      <c r="W22">
         <v>12131415</v>
       </c>
-      <c r="U22" t="s">
+      <c r="X22" t="s">
         <v>145</v>
       </c>
-      <c r="V22">
+      <c r="Y22">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1045</v>
       </c>
@@ -3280,53 +3550,65 @@
       <c r="G23">
         <v>4</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>11.2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>148.80000000000001</v>
+      </c>
+      <c r="K23" t="s">
         <v>315</v>
       </c>
-      <c r="I23" t="s">
+      <c r="L23" t="s">
         <v>147</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="K23" t="s">
+      <c r="N23" t="s">
         <v>59</v>
       </c>
-      <c r="L23" t="s">
+      <c r="O23" t="s">
         <v>27</v>
       </c>
-      <c r="M23" t="s">
+      <c r="P23" t="s">
         <v>67</v>
       </c>
-      <c r="N23">
+      <c r="Q23">
         <v>340</v>
       </c>
-      <c r="O23">
+      <c r="R23">
         <v>2</v>
       </c>
-      <c r="P23" t="s">
+      <c r="S23" t="s">
         <v>46</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="T23" t="s">
         <v>148</v>
       </c>
-      <c r="R23" t="s">
+      <c r="U23" t="s">
         <v>149</v>
       </c>
-      <c r="S23">
+      <c r="V23">
         <v>34590</v>
       </c>
-      <c r="T23">
+      <c r="W23">
         <v>13141516</v>
       </c>
-      <c r="U23" t="s">
+      <c r="X23" t="s">
         <v>150</v>
       </c>
-      <c r="V23">
+      <c r="Y23">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1046</v>
       </c>
@@ -3348,53 +3630,65 @@
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>251.1</v>
+      </c>
+      <c r="K24" t="s">
         <v>332</v>
       </c>
-      <c r="I24" t="s">
+      <c r="L24" t="s">
         <v>152</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="K24" t="s">
+      <c r="N24" t="s">
         <v>17</v>
       </c>
-      <c r="L24" t="s">
+      <c r="O24" t="s">
         <v>37</v>
       </c>
-      <c r="M24" t="s">
+      <c r="P24" t="s">
         <v>28</v>
       </c>
-      <c r="N24">
+      <c r="Q24">
         <v>165</v>
       </c>
-      <c r="O24">
+      <c r="R24">
         <v>3</v>
       </c>
-      <c r="P24" t="s">
+      <c r="S24" t="s">
         <v>61</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="T24" t="s">
         <v>153</v>
       </c>
-      <c r="R24" t="s">
+      <c r="U24" t="s">
         <v>154</v>
       </c>
-      <c r="S24">
+      <c r="V24">
         <v>45601</v>
       </c>
-      <c r="T24">
+      <c r="W24">
         <v>14151617</v>
       </c>
-      <c r="U24" t="s">
+      <c r="X24" t="s">
         <v>155</v>
       </c>
-      <c r="V24">
+      <c r="Y24">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1047</v>
       </c>
@@ -3416,53 +3710,65 @@
       <c r="G25">
         <v>6</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>7.5600000000000005</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>100.44</v>
+      </c>
+      <c r="K25" t="s">
         <v>312</v>
       </c>
-      <c r="I25" t="s">
+      <c r="L25" t="s">
         <v>157</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="K25" t="s">
+      <c r="N25" t="s">
         <v>26</v>
       </c>
-      <c r="L25" t="s">
+      <c r="O25" t="s">
         <v>18</v>
       </c>
-      <c r="M25" t="s">
+      <c r="P25" t="s">
         <v>19</v>
       </c>
-      <c r="N25">
+      <c r="Q25">
         <v>225</v>
       </c>
-      <c r="O25">
+      <c r="R25">
         <v>2</v>
       </c>
-      <c r="P25" t="s">
+      <c r="S25" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="T25" t="s">
         <v>158</v>
       </c>
-      <c r="R25" t="s">
+      <c r="U25" t="s">
         <v>159</v>
       </c>
-      <c r="S25">
+      <c r="V25">
         <v>56712</v>
       </c>
-      <c r="T25">
+      <c r="W25">
         <v>15161718</v>
       </c>
-      <c r="U25" t="s">
+      <c r="X25" t="s">
         <v>160</v>
       </c>
-      <c r="V25">
+      <c r="Y25">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1048</v>
       </c>
@@ -3484,53 +3790,65 @@
       <c r="G26">
         <v>5</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>20.299999999999997</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>269.7</v>
+      </c>
+      <c r="K26" t="s">
         <v>323</v>
       </c>
-      <c r="I26" t="s">
+      <c r="L26" t="s">
         <v>162</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="K26" t="s">
+      <c r="N26" t="s">
         <v>36</v>
       </c>
-      <c r="L26" t="s">
+      <c r="O26" t="s">
         <v>44</v>
       </c>
-      <c r="M26" t="s">
+      <c r="P26" t="s">
         <v>67</v>
       </c>
-      <c r="N26">
+      <c r="Q26">
         <v>310</v>
       </c>
-      <c r="O26">
+      <c r="R26">
         <v>5</v>
       </c>
-      <c r="P26" t="s">
+      <c r="S26" t="s">
         <v>29</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="T26" t="s">
         <v>163</v>
       </c>
-      <c r="R26" t="s">
+      <c r="U26" t="s">
         <v>164</v>
       </c>
-      <c r="S26">
+      <c r="V26">
         <v>67823</v>
       </c>
-      <c r="T26">
+      <c r="W26">
         <v>17181920</v>
       </c>
-      <c r="U26" t="s">
+      <c r="X26" t="s">
         <v>165</v>
       </c>
-      <c r="V26">
+      <c r="Y26">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1049</v>
       </c>
@@ -3552,53 +3870,65 @@
       <c r="G27">
         <v>2</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>11.9</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>158.1</v>
+      </c>
+      <c r="K27" t="s">
         <v>345</v>
       </c>
-      <c r="I27" t="s">
+      <c r="L27" t="s">
         <v>167</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="K27" t="s">
+      <c r="N27" t="s">
         <v>86</v>
       </c>
-      <c r="L27" t="s">
+      <c r="O27" t="s">
         <v>18</v>
       </c>
-      <c r="M27" t="s">
+      <c r="P27" t="s">
         <v>73</v>
       </c>
-      <c r="N27">
+      <c r="Q27">
         <v>275</v>
       </c>
-      <c r="O27">
+      <c r="R27">
         <v>4</v>
       </c>
-      <c r="P27" t="s">
+      <c r="S27" t="s">
         <v>46</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="T27" t="s">
         <v>168</v>
       </c>
-      <c r="R27" t="s">
+      <c r="U27" t="s">
         <v>169</v>
       </c>
-      <c r="S27">
+      <c r="V27">
         <v>78934</v>
       </c>
-      <c r="T27">
+      <c r="W27">
         <v>19202122</v>
       </c>
-      <c r="U27" t="s">
+      <c r="X27" t="s">
         <v>170</v>
       </c>
-      <c r="V27">
+      <c r="Y27">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1050</v>
       </c>
@@ -3620,53 +3950,65 @@
       <c r="G28">
         <v>1</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>15.4</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>204.6</v>
+      </c>
+      <c r="K28" t="s">
         <v>373</v>
       </c>
-      <c r="I28" t="s">
+      <c r="L28" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="K28" t="s">
+      <c r="N28" t="s">
         <v>52</v>
       </c>
-      <c r="L28" t="s">
+      <c r="O28" t="s">
         <v>27</v>
       </c>
-      <c r="M28" t="s">
+      <c r="P28" t="s">
         <v>28</v>
       </c>
-      <c r="N28">
+      <c r="Q28">
         <v>190</v>
       </c>
-      <c r="O28">
+      <c r="R28">
         <v>2</v>
       </c>
-      <c r="P28" t="s">
+      <c r="S28" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="T28" t="s">
         <v>173</v>
       </c>
-      <c r="R28" t="s">
+      <c r="U28" t="s">
         <v>174</v>
       </c>
-      <c r="S28">
+      <c r="V28">
         <v>89045</v>
       </c>
-      <c r="T28">
+      <c r="W28">
         <v>21222324</v>
       </c>
-      <c r="U28" t="s">
+      <c r="X28" t="s">
         <v>175</v>
       </c>
-      <c r="V28">
+      <c r="Y28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1052</v>
       </c>
@@ -3688,53 +4030,65 @@
       <c r="G29">
         <v>3</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>279</v>
+      </c>
+      <c r="K29" t="s">
         <v>318</v>
       </c>
-      <c r="I29" t="s">
+      <c r="L29" t="s">
         <v>177</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="K29" t="s">
+      <c r="N29" t="s">
         <v>59</v>
       </c>
-      <c r="L29" t="s">
+      <c r="O29" t="s">
         <v>37</v>
       </c>
-      <c r="M29" t="s">
+      <c r="P29" t="s">
         <v>67</v>
       </c>
-      <c r="N29">
+      <c r="Q29">
         <v>255</v>
       </c>
-      <c r="O29">
+      <c r="R29">
         <v>3</v>
       </c>
-      <c r="P29" t="s">
+      <c r="S29" t="s">
         <v>61</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="T29" t="s">
         <v>178</v>
       </c>
-      <c r="R29" t="s">
+      <c r="U29" t="s">
         <v>179</v>
       </c>
-      <c r="S29">
+      <c r="V29">
         <v>91267</v>
       </c>
-      <c r="T29">
+      <c r="W29">
         <v>25262728</v>
       </c>
-      <c r="U29" t="s">
+      <c r="X29" t="s">
         <v>180</v>
       </c>
-      <c r="V29">
+      <c r="Y29">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1053</v>
       </c>
@@ -3756,53 +4110,65 @@
       <c r="G30">
         <v>2</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>27.3</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>362.7</v>
+      </c>
+      <c r="K30" t="s">
         <v>378</v>
       </c>
-      <c r="I30" t="s">
+      <c r="L30" t="s">
         <v>182</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="K30" t="s">
+      <c r="N30" t="s">
         <v>86</v>
       </c>
-      <c r="L30" t="s">
+      <c r="O30" t="s">
         <v>44</v>
       </c>
-      <c r="M30" t="s">
+      <c r="P30" t="s">
         <v>28</v>
       </c>
-      <c r="N30">
+      <c r="Q30">
         <v>205</v>
       </c>
-      <c r="O30">
+      <c r="R30">
         <v>1</v>
       </c>
-      <c r="P30" t="s">
+      <c r="S30" t="s">
         <v>29</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="T30" t="s">
         <v>183</v>
       </c>
-      <c r="R30" t="s">
+      <c r="U30" t="s">
         <v>184</v>
       </c>
-      <c r="S30">
+      <c r="V30">
         <v>10278</v>
       </c>
-      <c r="T30">
+      <c r="W30">
         <v>27282930</v>
       </c>
-      <c r="U30" t="s">
+      <c r="X30" t="s">
         <v>185</v>
       </c>
-      <c r="V30">
+      <c r="Y30">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1054</v>
       </c>
@@ -3824,53 +4190,65 @@
       <c r="G31">
         <v>5</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>111.6</v>
+      </c>
+      <c r="K31" t="s">
         <v>312</v>
       </c>
-      <c r="I31" t="s">
+      <c r="L31" t="s">
         <v>187</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="K31" t="s">
+      <c r="N31" t="s">
         <v>17</v>
       </c>
-      <c r="L31" t="s">
+      <c r="O31" t="s">
         <v>27</v>
       </c>
-      <c r="M31" t="s">
+      <c r="P31" t="s">
         <v>73</v>
       </c>
-      <c r="N31">
+      <c r="Q31">
         <v>320</v>
       </c>
-      <c r="O31">
+      <c r="R31">
         <v>4</v>
       </c>
-      <c r="P31" t="s">
+      <c r="S31" t="s">
         <v>46</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="T31" t="s">
         <v>188</v>
       </c>
-      <c r="R31" t="s">
+      <c r="U31" t="s">
         <v>189</v>
       </c>
-      <c r="S31">
+      <c r="V31">
         <v>21389</v>
       </c>
-      <c r="T31">
+      <c r="W31">
         <v>29303132</v>
       </c>
-      <c r="U31" t="s">
+      <c r="X31" t="s">
         <v>190</v>
       </c>
-      <c r="V31">
+      <c r="Y31">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1055</v>
       </c>
@@ -3892,53 +4270,65 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>21.7</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>288.3</v>
+      </c>
+      <c r="K32" t="s">
         <v>345</v>
       </c>
-      <c r="I32" t="s">
+      <c r="L32" t="s">
         <v>192</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="K32" t="s">
+      <c r="N32" t="s">
         <v>26</v>
       </c>
-      <c r="L32" t="s">
+      <c r="O32" t="s">
         <v>44</v>
       </c>
-      <c r="M32" t="s">
+      <c r="P32" t="s">
         <v>53</v>
       </c>
-      <c r="N32">
+      <c r="Q32">
         <v>375</v>
       </c>
-      <c r="O32">
+      <c r="R32">
         <v>5</v>
       </c>
-      <c r="P32" t="s">
+      <c r="S32" t="s">
         <v>20</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="T32" t="s">
         <v>193</v>
       </c>
-      <c r="R32" t="s">
+      <c r="U32" t="s">
         <v>194</v>
       </c>
-      <c r="S32">
+      <c r="V32">
         <v>32490</v>
       </c>
-      <c r="T32">
+      <c r="W32">
         <v>31323334</v>
       </c>
-      <c r="U32" t="s">
+      <c r="X32" t="s">
         <v>195</v>
       </c>
-      <c r="V32">
+      <c r="Y32">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1056</v>
       </c>
@@ -3960,53 +4350,65 @@
       <c r="G33">
         <v>4</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>14.56</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>193.44</v>
+      </c>
+      <c r="K33" t="s">
         <v>323</v>
       </c>
-      <c r="I33" t="s">
+      <c r="L33" t="s">
         <v>197</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="K33" t="s">
+      <c r="N33" t="s">
         <v>36</v>
       </c>
-      <c r="L33" t="s">
+      <c r="O33" t="s">
         <v>18</v>
       </c>
-      <c r="M33" t="s">
+      <c r="P33" t="s">
         <v>67</v>
       </c>
-      <c r="N33">
+      <c r="Q33">
         <v>295</v>
       </c>
-      <c r="O33">
+      <c r="R33">
         <v>4</v>
       </c>
-      <c r="P33" t="s">
+      <c r="S33" t="s">
         <v>29</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="T33" t="s">
         <v>198</v>
       </c>
-      <c r="R33" t="s">
+      <c r="U33" t="s">
         <v>199</v>
       </c>
-      <c r="S33">
+      <c r="V33">
         <v>43501</v>
       </c>
-      <c r="T33">
+      <c r="W33">
         <v>33343536</v>
       </c>
-      <c r="U33" t="s">
+      <c r="X33" t="s">
         <v>200</v>
       </c>
-      <c r="V33">
+      <c r="Y33">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1057</v>
       </c>
@@ -4028,53 +4430,65 @@
       <c r="G34">
         <v>5</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>21.7</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>288.3</v>
+      </c>
+      <c r="K34" t="s">
         <v>312</v>
       </c>
-      <c r="I34" t="s">
+      <c r="L34" t="s">
         <v>202</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="K34" t="s">
+      <c r="N34" t="s">
         <v>52</v>
       </c>
-      <c r="L34" t="s">
+      <c r="O34" t="s">
         <v>37</v>
       </c>
-      <c r="M34" t="s">
+      <c r="P34" t="s">
         <v>73</v>
       </c>
-      <c r="N34">
+      <c r="Q34">
         <v>310</v>
       </c>
-      <c r="O34">
+      <c r="R34">
         <v>3</v>
       </c>
-      <c r="P34" t="s">
+      <c r="S34" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="T34" t="s">
         <v>203</v>
       </c>
-      <c r="R34" t="s">
+      <c r="U34" t="s">
         <v>204</v>
       </c>
-      <c r="S34">
+      <c r="V34">
         <v>54612</v>
       </c>
-      <c r="T34">
+      <c r="W34">
         <v>35363738</v>
       </c>
-      <c r="U34" t="s">
+      <c r="X34" t="s">
         <v>205</v>
       </c>
-      <c r="V34">
+      <c r="Y34">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1058</v>
       </c>
@@ -4096,53 +4510,65 @@
       <c r="G35">
         <v>3</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>9.24</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>122.76</v>
+      </c>
+      <c r="K35" t="s">
         <v>345</v>
       </c>
-      <c r="I35" t="s">
+      <c r="L35" t="s">
         <v>207</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="K35" t="s">
+      <c r="N35" t="s">
         <v>59</v>
       </c>
-      <c r="L35" t="s">
+      <c r="O35" t="s">
         <v>18</v>
       </c>
-      <c r="M35" t="s">
+      <c r="P35" t="s">
         <v>53</v>
       </c>
-      <c r="N35">
+      <c r="Q35">
         <v>210</v>
       </c>
-      <c r="O35">
+      <c r="R35">
         <v>3</v>
       </c>
-      <c r="P35" t="s">
+      <c r="S35" t="s">
         <v>46</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="T35" t="s">
         <v>208</v>
       </c>
-      <c r="R35" t="s">
+      <c r="U35" t="s">
         <v>209</v>
       </c>
-      <c r="S35">
+      <c r="V35">
         <v>65723</v>
       </c>
-      <c r="T35">
+      <c r="W35">
         <v>37383940</v>
       </c>
-      <c r="U35" t="s">
+      <c r="X35" t="s">
         <v>210</v>
       </c>
-      <c r="V35">
+      <c r="Y35">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1059</v>
       </c>
@@ -4164,53 +4590,65 @@
       <c r="G36">
         <v>4</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>13.44</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>178.56</v>
+      </c>
+      <c r="K36" t="s">
         <v>315</v>
       </c>
-      <c r="I36" t="s">
+      <c r="L36" t="s">
         <v>212</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="K36" t="s">
+      <c r="N36" t="s">
         <v>86</v>
       </c>
-      <c r="L36" t="s">
+      <c r="O36" t="s">
         <v>27</v>
       </c>
-      <c r="M36" t="s">
+      <c r="P36" t="s">
         <v>28</v>
       </c>
-      <c r="N36">
+      <c r="Q36">
         <v>170</v>
       </c>
-      <c r="O36">
+      <c r="R36">
         <v>2</v>
       </c>
-      <c r="P36" t="s">
+      <c r="S36" t="s">
         <v>20</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="T36" t="s">
         <v>213</v>
       </c>
-      <c r="R36" t="s">
+      <c r="U36" t="s">
         <v>214</v>
       </c>
-      <c r="S36">
+      <c r="V36">
         <v>76834</v>
       </c>
-      <c r="T36">
+      <c r="W36">
         <v>39404142</v>
       </c>
-      <c r="U36" t="s">
+      <c r="X36" t="s">
         <v>215</v>
       </c>
-      <c r="V36">
+      <c r="Y36">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1060</v>
       </c>
@@ -4232,53 +4670,65 @@
       <c r="G37">
         <v>2</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>12.32</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>163.68</v>
+      </c>
+      <c r="K37" t="s">
         <v>378</v>
       </c>
-      <c r="I37" t="s">
+      <c r="L37" t="s">
         <v>217</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="K37" t="s">
+      <c r="N37" t="s">
         <v>17</v>
       </c>
-      <c r="L37" t="s">
+      <c r="O37" t="s">
         <v>44</v>
       </c>
-      <c r="M37" t="s">
+      <c r="P37" t="s">
         <v>73</v>
       </c>
-      <c r="N37">
+      <c r="Q37">
         <v>265</v>
       </c>
-      <c r="O37">
+      <c r="R37">
         <v>3</v>
       </c>
-      <c r="P37" t="s">
+      <c r="S37" t="s">
         <v>61</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="T37" t="s">
         <v>218</v>
       </c>
-      <c r="R37" t="s">
+      <c r="U37" t="s">
         <v>219</v>
       </c>
-      <c r="S37">
+      <c r="V37">
         <v>87945</v>
       </c>
-      <c r="T37">
+      <c r="W37">
         <v>41424344</v>
       </c>
-      <c r="U37" t="s">
+      <c r="X37" t="s">
         <v>220</v>
       </c>
-      <c r="V37">
+      <c r="Y37">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1061</v>
       </c>
@@ -4300,53 +4750,65 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>14.7</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>195.3</v>
+      </c>
+      <c r="K38" t="s">
         <v>318</v>
       </c>
-      <c r="I38" t="s">
+      <c r="L38" t="s">
         <v>222</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K38" t="s">
+      <c r="N38" t="s">
         <v>36</v>
       </c>
-      <c r="L38" t="s">
+      <c r="O38" t="s">
         <v>27</v>
       </c>
-      <c r="M38" t="s">
+      <c r="P38" t="s">
         <v>19</v>
       </c>
-      <c r="N38">
+      <c r="Q38">
         <v>220</v>
       </c>
-      <c r="O38">
+      <c r="R38">
         <v>1</v>
       </c>
-      <c r="P38" t="s">
+      <c r="S38" t="s">
         <v>46</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="T38" t="s">
         <v>223</v>
       </c>
-      <c r="R38" t="s">
+      <c r="U38" t="s">
         <v>224</v>
       </c>
-      <c r="S38">
+      <c r="V38">
         <v>89016</v>
       </c>
-      <c r="T38">
+      <c r="W38">
         <v>43454748</v>
       </c>
-      <c r="U38" t="s">
+      <c r="X38" t="s">
         <v>225</v>
       </c>
-      <c r="V38">
+      <c r="Y38">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1062</v>
       </c>
@@ -4368,53 +4830,65 @@
       <c r="G39">
         <v>3</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>14.700000000000001</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>195.3</v>
+      </c>
+      <c r="K39" t="s">
         <v>397</v>
       </c>
-      <c r="I39" t="s">
+      <c r="L39" t="s">
         <v>227</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="K39" t="s">
+      <c r="N39" t="s">
         <v>52</v>
       </c>
-      <c r="L39" t="s">
+      <c r="O39" t="s">
         <v>18</v>
       </c>
-      <c r="M39" t="s">
+      <c r="P39" t="s">
         <v>53</v>
       </c>
-      <c r="N39">
+      <c r="Q39">
         <v>390</v>
       </c>
-      <c r="O39">
+      <c r="R39">
         <v>4</v>
       </c>
-      <c r="P39" t="s">
+      <c r="S39" t="s">
         <v>20</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="T39" t="s">
         <v>228</v>
       </c>
-      <c r="R39" t="s">
+      <c r="U39" t="s">
         <v>229</v>
       </c>
-      <c r="S39">
+      <c r="V39">
         <v>90127</v>
       </c>
-      <c r="T39">
+      <c r="W39">
         <v>49505152</v>
       </c>
-      <c r="U39" t="s">
+      <c r="X39" t="s">
         <v>230</v>
       </c>
-      <c r="V39">
+      <c r="Y39">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1063</v>
       </c>
@@ -4436,53 +4910,65 @@
       <c r="G40">
         <v>2</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>16.8</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="2"/>
+        <v>223.2</v>
+      </c>
+      <c r="K40" t="s">
         <v>345</v>
       </c>
-      <c r="I40" t="s">
+      <c r="L40" t="s">
         <v>232</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="K40" t="s">
+      <c r="N40" t="s">
         <v>26</v>
       </c>
-      <c r="L40" t="s">
+      <c r="O40" t="s">
         <v>37</v>
       </c>
-      <c r="M40" t="s">
+      <c r="P40" t="s">
         <v>67</v>
       </c>
-      <c r="N40">
+      <c r="Q40">
         <v>310</v>
       </c>
-      <c r="O40">
+      <c r="R40">
         <v>1</v>
       </c>
-      <c r="P40" t="s">
+      <c r="S40" t="s">
         <v>29</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="T40" t="s">
         <v>233</v>
       </c>
-      <c r="R40" t="s">
+      <c r="U40" t="s">
         <v>234</v>
       </c>
-      <c r="S40">
+      <c r="V40">
         <v>91238</v>
       </c>
-      <c r="T40">
+      <c r="W40">
         <v>51535754</v>
       </c>
-      <c r="U40" t="s">
+      <c r="X40" t="s">
         <v>235</v>
       </c>
-      <c r="V40">
+      <c r="Y40">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1064</v>
       </c>
@@ -4504,53 +4990,65 @@
       <c r="G41">
         <v>1</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>7.35</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="2"/>
+        <v>97.65</v>
+      </c>
+      <c r="K41" t="s">
         <v>402</v>
       </c>
-      <c r="I41" t="s">
+      <c r="L41" t="s">
         <v>237</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="K41" t="s">
+      <c r="N41" t="s">
         <v>86</v>
       </c>
-      <c r="L41" t="s">
+      <c r="O41" t="s">
         <v>18</v>
       </c>
-      <c r="M41" t="s">
+      <c r="P41" t="s">
         <v>28</v>
       </c>
-      <c r="N41">
+      <c r="Q41">
         <v>215</v>
       </c>
-      <c r="O41">
+      <c r="R41">
         <v>5</v>
       </c>
-      <c r="P41" t="s">
+      <c r="S41" t="s">
         <v>61</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="T41" t="s">
         <v>238</v>
       </c>
-      <c r="R41" t="s">
+      <c r="U41" t="s">
         <v>239</v>
       </c>
-      <c r="S41">
+      <c r="V41">
         <v>92349</v>
       </c>
-      <c r="T41">
+      <c r="W41">
         <v>57596162</v>
       </c>
-      <c r="U41" t="s">
+      <c r="X41" t="s">
         <v>240</v>
       </c>
-      <c r="V41">
+      <c r="Y41">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1065</v>
       </c>
@@ -4572,53 +5070,65 @@
       <c r="G42">
         <v>2</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="2"/>
+        <v>213.9</v>
+      </c>
+      <c r="K42" t="s">
         <v>323</v>
       </c>
-      <c r="I42" t="s">
+      <c r="L42" t="s">
         <v>242</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="K42" t="s">
+      <c r="N42" t="s">
         <v>59</v>
       </c>
-      <c r="L42" t="s">
+      <c r="O42" t="s">
         <v>44</v>
       </c>
-      <c r="M42" t="s">
+      <c r="P42" t="s">
         <v>73</v>
       </c>
-      <c r="N42">
+      <c r="Q42">
         <v>295</v>
       </c>
-      <c r="O42">
+      <c r="R42">
         <v>2</v>
       </c>
-      <c r="P42" t="s">
+      <c r="S42" t="s">
         <v>20</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="T42" t="s">
         <v>243</v>
       </c>
-      <c r="R42" t="s">
+      <c r="U42" t="s">
         <v>244</v>
       </c>
-      <c r="S42">
+      <c r="V42">
         <v>93450</v>
       </c>
-      <c r="T42">
+      <c r="W42">
         <v>63677172</v>
       </c>
-      <c r="U42" t="s">
+      <c r="X42" t="s">
         <v>245</v>
       </c>
-      <c r="V42">
+      <c r="Y42">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1066</v>
       </c>
@@ -4640,53 +5150,65 @@
       <c r="G43">
         <v>3</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>9.66</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="2"/>
+        <v>128.34</v>
+      </c>
+      <c r="K43" t="s">
         <v>315</v>
       </c>
-      <c r="I43" t="s">
+      <c r="L43" t="s">
         <v>247</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="K43" t="s">
+      <c r="N43" t="s">
         <v>17</v>
       </c>
-      <c r="L43" t="s">
+      <c r="O43" t="s">
         <v>18</v>
       </c>
-      <c r="M43" t="s">
+      <c r="P43" t="s">
         <v>67</v>
       </c>
-      <c r="N43">
+      <c r="Q43">
         <v>240</v>
       </c>
-      <c r="O43">
+      <c r="R43">
         <v>4</v>
       </c>
-      <c r="P43" t="s">
+      <c r="S43" t="s">
         <v>46</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="T43" t="s">
         <v>248</v>
       </c>
-      <c r="R43" t="s">
+      <c r="U43" t="s">
         <v>249</v>
       </c>
-      <c r="S43">
+      <c r="V43">
         <v>94561</v>
       </c>
-      <c r="T43">
+      <c r="W43">
         <v>73758182</v>
       </c>
-      <c r="U43" t="s">
+      <c r="X43" t="s">
         <v>250</v>
       </c>
-      <c r="V43">
+      <c r="Y43">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1067</v>
       </c>
@@ -4708,53 +5230,65 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>20.3</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="2"/>
+        <v>269.7</v>
+      </c>
+      <c r="K44" t="s">
         <v>412</v>
       </c>
-      <c r="I44" t="s">
+      <c r="L44" t="s">
         <v>252</v>
       </c>
-      <c r="J44" s="1">
+      <c r="M44" s="1">
         <v>12</v>
       </c>
-      <c r="K44" t="s">
+      <c r="N44" t="s">
         <v>26</v>
       </c>
-      <c r="L44" t="s">
+      <c r="O44" t="s">
         <v>27</v>
       </c>
-      <c r="M44" t="s">
+      <c r="P44" t="s">
         <v>28</v>
       </c>
-      <c r="N44">
+      <c r="Q44">
         <v>120</v>
       </c>
-      <c r="O44">
+      <c r="R44">
         <v>1</v>
       </c>
-      <c r="P44" t="s">
+      <c r="S44" t="s">
         <v>29</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="T44" t="s">
         <v>253</v>
       </c>
-      <c r="R44" t="s">
+      <c r="U44" t="s">
         <v>254</v>
       </c>
-      <c r="S44">
+      <c r="V44">
         <v>95672</v>
       </c>
-      <c r="T44">
+      <c r="W44">
         <v>79819292</v>
       </c>
-      <c r="U44" t="s">
+      <c r="X44" t="s">
         <v>255</v>
       </c>
-      <c r="V44">
+      <c r="Y44">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1068</v>
       </c>
@@ -4776,53 +5310,65 @@
       <c r="G45">
         <v>5</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>7.7</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="2"/>
+        <v>102.3</v>
+      </c>
+      <c r="K45" t="s">
         <v>345</v>
       </c>
-      <c r="I45" t="s">
+      <c r="L45" t="s">
         <v>257</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="K45" t="s">
+      <c r="N45" t="s">
         <v>36</v>
       </c>
-      <c r="L45" t="s">
+      <c r="O45" t="s">
         <v>37</v>
       </c>
-      <c r="M45" t="s">
+      <c r="P45" t="s">
         <v>53</v>
       </c>
-      <c r="N45">
+      <c r="Q45">
         <v>180</v>
       </c>
-      <c r="O45">
+      <c r="R45">
         <v>5</v>
       </c>
-      <c r="P45" t="s">
+      <c r="S45" t="s">
         <v>61</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="T45" t="s">
         <v>258</v>
       </c>
-      <c r="R45" t="s">
+      <c r="U45" t="s">
         <v>259</v>
       </c>
-      <c r="S45">
+      <c r="V45">
         <v>96783</v>
       </c>
-      <c r="T45">
+      <c r="W45">
         <v>81831002</v>
       </c>
-      <c r="U45" t="s">
+      <c r="X45" t="s">
         <v>260</v>
       </c>
-      <c r="V45">
+      <c r="Y45">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1069</v>
       </c>
@@ -4844,53 +5390,65 @@
       <c r="G46">
         <v>4</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>17.64</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="2"/>
+        <v>234.36</v>
+      </c>
+      <c r="K46" t="s">
         <v>323</v>
       </c>
-      <c r="I46" t="s">
+      <c r="L46" t="s">
         <v>262</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="K46" t="s">
+      <c r="N46" t="s">
         <v>17</v>
       </c>
-      <c r="L46" t="s">
+      <c r="O46" t="s">
         <v>44</v>
       </c>
-      <c r="M46" t="s">
+      <c r="P46" t="s">
         <v>67</v>
       </c>
-      <c r="N46">
+      <c r="Q46">
         <v>260</v>
       </c>
-      <c r="O46">
+      <c r="R46">
         <v>3</v>
       </c>
-      <c r="P46" t="s">
+      <c r="S46" t="s">
         <v>20</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="T46" t="s">
         <v>263</v>
       </c>
-      <c r="R46" t="s">
+      <c r="U46" t="s">
         <v>264</v>
       </c>
-      <c r="S46">
+      <c r="V46">
         <v>97894</v>
       </c>
-      <c r="T46">
+      <c r="W46">
         <v>83841112</v>
       </c>
-      <c r="U46" t="s">
+      <c r="X46" t="s">
         <v>265</v>
       </c>
-      <c r="V46">
+      <c r="Y46">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1070</v>
       </c>
@@ -4912,53 +5470,65 @@
       <c r="G47">
         <v>2</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>12.88</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="2"/>
+        <v>171.12</v>
+      </c>
+      <c r="K47" t="s">
         <v>318</v>
       </c>
-      <c r="I47" t="s">
+      <c r="L47" t="s">
         <v>267</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="K47" t="s">
+      <c r="N47" t="s">
         <v>52</v>
       </c>
-      <c r="L47" t="s">
+      <c r="O47" t="s">
         <v>18</v>
       </c>
-      <c r="M47" t="s">
+      <c r="P47" t="s">
         <v>19</v>
       </c>
-      <c r="N47">
+      <c r="Q47">
         <v>300</v>
       </c>
-      <c r="O47">
+      <c r="R47">
         <v>2</v>
       </c>
-      <c r="P47" t="s">
+      <c r="S47" t="s">
         <v>46</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="T47" t="s">
         <v>268</v>
       </c>
-      <c r="R47" t="s">
+      <c r="U47" t="s">
         <v>269</v>
       </c>
-      <c r="S47">
+      <c r="V47">
         <v>98905</v>
       </c>
-      <c r="T47">
+      <c r="W47">
         <v>84851222</v>
       </c>
-      <c r="U47" t="s">
+      <c r="X47" t="s">
         <v>270</v>
       </c>
-      <c r="V47">
+      <c r="Y47">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1071</v>
       </c>
@@ -4980,53 +5550,65 @@
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>235</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>16.45</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="2"/>
+        <v>218.55</v>
+      </c>
+      <c r="K48" t="s">
         <v>373</v>
       </c>
-      <c r="I48" t="s">
+      <c r="L48" t="s">
         <v>272</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="M48" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="K48" t="s">
+      <c r="N48" t="s">
         <v>59</v>
       </c>
-      <c r="L48" t="s">
+      <c r="O48" t="s">
         <v>27</v>
       </c>
-      <c r="M48" t="s">
+      <c r="P48" t="s">
         <v>67</v>
       </c>
-      <c r="N48">
+      <c r="Q48">
         <v>250</v>
       </c>
-      <c r="O48">
+      <c r="R48">
         <v>2</v>
       </c>
-      <c r="P48" t="s">
+      <c r="S48" t="s">
         <v>61</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="T48" t="s">
         <v>273</v>
       </c>
-      <c r="R48" t="s">
+      <c r="U48" t="s">
         <v>274</v>
       </c>
-      <c r="S48">
+      <c r="V48">
         <v>99016</v>
       </c>
-      <c r="T48">
+      <c r="W48">
         <v>85861332</v>
       </c>
-      <c r="U48" t="s">
+      <c r="X48" t="s">
         <v>275</v>
       </c>
-      <c r="V48">
+      <c r="Y48">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1072</v>
       </c>
@@ -5048,53 +5630,65 @@
       <c r="G49">
         <v>3</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>23.1</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="2"/>
+        <v>306.89999999999998</v>
+      </c>
+      <c r="K49" t="s">
         <v>318</v>
       </c>
-      <c r="I49" t="s">
+      <c r="L49" t="s">
         <v>277</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="K49" t="s">
+      <c r="N49" t="s">
         <v>26</v>
       </c>
-      <c r="L49" t="s">
+      <c r="O49" t="s">
         <v>37</v>
       </c>
-      <c r="M49" t="s">
+      <c r="P49" t="s">
         <v>53</v>
       </c>
-      <c r="N49">
+      <c r="Q49">
         <v>320</v>
       </c>
-      <c r="O49">
+      <c r="R49">
         <v>5</v>
       </c>
-      <c r="P49" t="s">
+      <c r="S49" t="s">
         <v>29</v>
       </c>
-      <c r="Q49" t="s">
+      <c r="T49" t="s">
         <v>278</v>
       </c>
-      <c r="R49" t="s">
+      <c r="U49" t="s">
         <v>279</v>
       </c>
-      <c r="S49">
+      <c r="V49">
         <v>90127</v>
       </c>
-      <c r="T49">
+      <c r="W49">
         <v>86871442</v>
       </c>
-      <c r="U49" t="s">
+      <c r="X49" t="s">
         <v>280</v>
       </c>
-      <c r="V49">
+      <c r="Y49">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1073</v>
       </c>
@@ -5116,53 +5710,65 @@
       <c r="G50">
         <v>2</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>28.7</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="2"/>
+        <v>381.3</v>
+      </c>
+      <c r="K50" t="s">
         <v>332</v>
       </c>
-      <c r="I50" t="s">
+      <c r="L50" t="s">
         <v>282</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="K50" t="s">
+      <c r="N50" t="s">
         <v>36</v>
       </c>
-      <c r="L50" t="s">
+      <c r="O50" t="s">
         <v>18</v>
       </c>
-      <c r="M50" t="s">
+      <c r="P50" t="s">
         <v>28</v>
       </c>
-      <c r="N50">
+      <c r="Q50">
         <v>290</v>
       </c>
-      <c r="O50">
+      <c r="R50">
         <v>2</v>
       </c>
-      <c r="P50" t="s">
+      <c r="S50" t="s">
         <v>61</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="T50" t="s">
         <v>283</v>
       </c>
-      <c r="R50" t="s">
+      <c r="U50" t="s">
         <v>284</v>
       </c>
-      <c r="S50">
+      <c r="V50">
         <v>91238</v>
       </c>
-      <c r="T50">
+      <c r="W50">
         <v>87881552</v>
       </c>
-      <c r="U50" t="s">
+      <c r="X50" t="s">
         <v>285</v>
       </c>
-      <c r="V50">
+      <c r="Y50">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1074</v>
       </c>
@@ -5184,53 +5790,65 @@
       <c r="G51">
         <v>6</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>174</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>12.18</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="2"/>
+        <v>161.82</v>
+      </c>
+      <c r="K51" t="s">
         <v>412</v>
       </c>
-      <c r="I51" t="s">
+      <c r="L51" t="s">
         <v>287</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="K51" t="s">
+      <c r="N51" t="s">
         <v>86</v>
       </c>
-      <c r="L51" t="s">
+      <c r="O51" t="s">
         <v>27</v>
       </c>
-      <c r="M51" t="s">
+      <c r="P51" t="s">
         <v>67</v>
       </c>
-      <c r="N51">
+      <c r="Q51">
         <v>350</v>
       </c>
-      <c r="O51">
+      <c r="R51">
         <v>1</v>
       </c>
-      <c r="P51" t="s">
+      <c r="S51" t="s">
         <v>20</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="T51" t="s">
         <v>288</v>
       </c>
-      <c r="R51" t="s">
+      <c r="U51" t="s">
         <v>289</v>
       </c>
-      <c r="S51">
+      <c r="V51">
         <v>92349</v>
       </c>
-      <c r="T51">
+      <c r="W51">
         <v>88891662</v>
       </c>
-      <c r="U51" t="s">
+      <c r="X51" t="s">
         <v>290</v>
       </c>
-      <c r="V51">
+      <c r="Y51">
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1075</v>
       </c>
@@ -5252,53 +5870,65 @@
       <c r="G52">
         <v>1</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>22.75</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>302.25</v>
+      </c>
+      <c r="K52" t="s">
         <v>345</v>
       </c>
-      <c r="I52" t="s">
+      <c r="L52" t="s">
         <v>292</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="M52" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="K52" t="s">
+      <c r="N52" t="s">
         <v>17</v>
       </c>
-      <c r="L52" t="s">
+      <c r="O52" t="s">
         <v>37</v>
       </c>
-      <c r="M52" t="s">
+      <c r="P52" t="s">
         <v>73</v>
       </c>
-      <c r="N52">
+      <c r="Q52">
         <v>210</v>
       </c>
-      <c r="O52">
+      <c r="R52">
         <v>1</v>
       </c>
-      <c r="P52" t="s">
+      <c r="S52" t="s">
         <v>29</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="T52" t="s">
         <v>293</v>
       </c>
-      <c r="R52" t="s">
+      <c r="U52" t="s">
         <v>294</v>
       </c>
-      <c r="S52">
+      <c r="V52">
         <v>93450</v>
       </c>
-      <c r="T52">
+      <c r="W52">
         <v>89901772</v>
       </c>
-      <c r="U52" t="s">
+      <c r="X52" t="s">
         <v>295</v>
       </c>
-      <c r="V52">
+      <c r="Y52">
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1076</v>
       </c>
@@ -5320,53 +5950,65 @@
       <c r="G53">
         <v>3</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>11.97</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="2"/>
+        <v>159.03</v>
+      </c>
+      <c r="K53" t="s">
         <v>323</v>
       </c>
-      <c r="I53" t="s">
+      <c r="L53" t="s">
         <v>297</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="K53" t="s">
+      <c r="N53" t="s">
         <v>52</v>
       </c>
-      <c r="L53" t="s">
+      <c r="O53" t="s">
         <v>27</v>
       </c>
-      <c r="M53" t="s">
+      <c r="P53" t="s">
         <v>19</v>
       </c>
-      <c r="N53">
+      <c r="Q53">
         <v>280</v>
       </c>
-      <c r="O53">
+      <c r="R53">
         <v>4</v>
       </c>
-      <c r="P53" t="s">
+      <c r="S53" t="s">
         <v>46</v>
       </c>
-      <c r="Q53" t="s">
+      <c r="T53" t="s">
         <v>298</v>
       </c>
-      <c r="R53" t="s">
+      <c r="U53" t="s">
         <v>299</v>
       </c>
-      <c r="S53">
+      <c r="V53">
         <v>94561</v>
       </c>
-      <c r="T53">
+      <c r="W53">
         <v>90911882</v>
       </c>
-      <c r="U53" t="s">
+      <c r="X53" t="s">
         <v>300</v>
       </c>
-      <c r="V53">
+      <c r="Y53">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1077</v>
       </c>
@@ -5388,53 +6030,65 @@
       <c r="G54">
         <v>4</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>272</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>19.04</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="2"/>
+        <v>252.96</v>
+      </c>
+      <c r="K54" t="s">
         <v>318</v>
       </c>
-      <c r="I54" t="s">
+      <c r="L54" t="s">
         <v>302</v>
       </c>
-      <c r="J54" s="1">
+      <c r="M54" s="1">
         <v>5</v>
       </c>
-      <c r="K54" t="s">
+      <c r="N54" t="s">
         <v>59</v>
       </c>
-      <c r="L54" t="s">
+      <c r="O54" t="s">
         <v>18</v>
       </c>
-      <c r="M54" t="s">
+      <c r="P54" t="s">
         <v>67</v>
       </c>
-      <c r="N54">
+      <c r="Q54">
         <v>180</v>
       </c>
-      <c r="O54">
+      <c r="R54">
         <v>4</v>
       </c>
-      <c r="P54" t="s">
+      <c r="S54" t="s">
         <v>61</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="T54" t="s">
         <v>303</v>
       </c>
-      <c r="R54" t="s">
+      <c r="U54" t="s">
         <v>304</v>
       </c>
-      <c r="S54">
+      <c r="V54">
         <v>95672</v>
       </c>
-      <c r="T54">
+      <c r="W54">
         <v>91921992</v>
       </c>
-      <c r="U54" t="s">
+      <c r="X54" t="s">
         <v>305</v>
       </c>
-      <c r="V54">
+      <c r="Y54">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1078</v>
       </c>
@@ -5456,49 +6110,61 @@
       <c r="G55">
         <v>2</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>6.86</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="2"/>
+        <v>91.14</v>
+      </c>
+      <c r="K55" t="s">
         <v>360</v>
       </c>
-      <c r="I55" t="s">
+      <c r="L55" t="s">
         <v>307</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="M55" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="K55" t="s">
+      <c r="N55" t="s">
         <v>36</v>
       </c>
-      <c r="L55" t="s">
+      <c r="O55" t="s">
         <v>44</v>
       </c>
-      <c r="M55" t="s">
+      <c r="P55" t="s">
         <v>73</v>
       </c>
-      <c r="N55">
+      <c r="Q55">
         <v>230</v>
       </c>
-      <c r="O55">
+      <c r="R55">
         <v>5</v>
       </c>
-      <c r="P55" t="s">
+      <c r="S55" t="s">
         <v>20</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="T55" t="s">
         <v>308</v>
       </c>
-      <c r="R55" t="s">
+      <c r="U55" t="s">
         <v>309</v>
       </c>
-      <c r="S55">
+      <c r="V55">
         <v>96783</v>
       </c>
-      <c r="T55">
+      <c r="W55">
         <v>92932002</v>
       </c>
-      <c r="U55" t="s">
+      <c r="X55" t="s">
         <v>310</v>
       </c>
-      <c r="V55">
+      <c r="Y55">
         <v>28</v>
       </c>
     </row>
@@ -5508,6 +6174,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Status xmlns="2aed4346-8012-4133-9837-e496d0f5c99a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EAC3B332A2FD04E918F9FD72E2B30AC" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="44c88873497b10f3ff10f19c7c5db422">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aed4346-8012-4133-9837-e496d0f5c99a" xmlns:ns3="15179a99-4cef-4bac-ab20-a4c03d7ec5db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c5bd0a3e89f1d34ce551ea40c27f6bd8" ns2:_="" ns3:_="">
     <xsd:import namespace="2aed4346-8012-4133-9837-e496d0f5c99a"/>
@@ -5738,35 +6425,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="15179a99-4cef-4bac-ab20-a4c03d7ec5db" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2aed4346-8012-4133-9837-e496d0f5c99a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Status xmlns="2aed4346-8012-4133-9837-e496d0f5c99a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DD313B-1E33-4FD8-8AD5-A610EC26773D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C86A4E6-ACF0-45C6-A914-9712D4CC78BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
+    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5FCFB79-8449-4D5C-843D-F375C8BA3EEA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5FCFB79-8449-4D5C-843D-F375C8BA3EEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C86A4E6-ACF0-45C6-A914-9712D4CC78BA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DD313B-1E33-4FD8-8AD5-A610EC26773D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2aed4346-8012-4133-9837-e496d0f5c99a"/>
+    <ds:schemaRef ds:uri="15179a99-4cef-4bac-ab20-a4c03d7ec5db"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tailwind - calculation - done!
</commit_message>
<xml_diff>
--- a/Tailwind-Traders-Sales.xlsx
+++ b/Tailwind-Traders-Sales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Courses\Coursera\Microsoft Power BI Data Analyst Professional Certificate\Microsoft Power BI Data Analyst Professional Certificate\POWER BI\Capstone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66550900-4719-440E-B1FC-67B051E1C895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71377D15-4500-417F-9E3E-64D6017059D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
@@ -1440,8 +1440,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1469,9 +1477,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1755,7 +1765,7 @@
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD10"/>
+      <selection sqref="A1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,79 +1782,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6186,15 +6196,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EAC3B332A2FD04E918F9FD72E2B30AC" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="44c88873497b10f3ff10f19c7c5db422">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aed4346-8012-4133-9837-e496d0f5c99a" xmlns:ns3="15179a99-4cef-4bac-ab20-a4c03d7ec5db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c5bd0a3e89f1d34ce551ea40c27f6bd8" ns2:_="" ns3:_="">
     <xsd:import namespace="2aed4346-8012-4133-9837-e496d0f5c99a"/>
@@ -6425,6 +6426,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C86A4E6-ACF0-45C6-A914-9712D4CC78BA}">
   <ds:schemaRefs>
@@ -6437,14 +6447,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5FCFB79-8449-4D5C-843D-F375C8BA3EEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42DD313B-1E33-4FD8-8AD5-A610EC26773D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6461,4 +6463,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5FCFB79-8449-4D5C-843D-F375C8BA3EEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>